<commit_message>
checked for formatting consistency
</commit_message>
<xml_diff>
--- a/data/supplementaryRawDataTables.xlsx
+++ b/data/supplementaryRawDataTables.xlsx
@@ -5,10 +5,10 @@
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rb_ja\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rb_ja\OneDrive\CSL LAB\GITHUB SYNC\DigitEyes\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D07DBCF7-765D-4A2A-9526-51245EC9106A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{D07DBCF7-765D-4A2A-9526-51245EC9106A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{BDEC4E2E-85EC-46F6-9C63-CFEAC159BE04}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -759,7 +759,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="110">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -823,47 +823,221 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -871,38 +1045,11 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -910,185 +1057,41 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -1193,8 +1196,8 @@
       <xdr:rowOff>557212</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1704954" cy="168829"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -1392,7 +1395,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -1505,8 +1508,8 @@
       <xdr:rowOff>566738</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1735988" cy="168829"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -1704,7 +1707,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -1817,8 +1820,8 @@
       <xdr:rowOff>700089</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1761636" cy="168829"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -2016,7 +2019,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -2129,8 +2132,8 @@
       <xdr:rowOff>633412</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1761636" cy="168829"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -2328,7 +2331,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -2441,8 +2444,8 @@
       <xdr:rowOff>571500</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1761636" cy="168829"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -2640,7 +2643,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -3835,23 +3838,23 @@
     <col min="13" max="256" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="32" customFormat="1" ht="32.25" customHeight="1">
+    <row r="1" spans="1:12" s="30" customFormat="1" ht="32.25" customHeight="1">
       <c r="A1" s="2"/>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="81" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="64"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-    </row>
-    <row r="2" spans="1:12" s="32" customFormat="1" ht="20.25" customHeight="1">
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+    </row>
+    <row r="2" spans="1:12" s="30" customFormat="1" ht="20.25" customHeight="1">
       <c r="A2" s="3"/>
       <c r="B2" s="4">
         <v>2.5000000000000001E-2</v>
@@ -3862,10 +3865,10 @@
       <c r="D2" s="6">
         <v>0.97499999999999998</v>
       </c>
-      <c r="E2" s="25"/>
-      <c r="F2" s="65"/>
-    </row>
-    <row r="3" spans="1:12" s="32" customFormat="1" ht="20" customHeight="1">
+      <c r="E2" s="23"/>
+      <c r="F2" s="54"/>
+    </row>
+    <row r="3" spans="1:12" s="30" customFormat="1" ht="20" customHeight="1">
       <c r="A3" s="7" t="s">
         <v>42</v>
       </c>
@@ -3878,10 +3881,10 @@
       <c r="D3" s="10">
         <v>70.102306200000001</v>
       </c>
-      <c r="E3" s="26"/>
-      <c r="F3" s="65"/>
-    </row>
-    <row r="4" spans="1:12" s="32" customFormat="1" ht="20" customHeight="1">
+      <c r="E3" s="24"/>
+      <c r="F3" s="54"/>
+    </row>
+    <row r="4" spans="1:12" s="30" customFormat="1" ht="20" customHeight="1">
       <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
@@ -3894,10 +3897,10 @@
       <c r="D4" s="10">
         <v>-0.79102729999999999</v>
       </c>
-      <c r="E4" s="26"/>
-      <c r="F4" s="65"/>
-    </row>
-    <row r="5" spans="1:12" s="32" customFormat="1" ht="20" customHeight="1">
+      <c r="E4" s="24"/>
+      <c r="F4" s="54"/>
+    </row>
+    <row r="5" spans="1:12" s="30" customFormat="1" ht="20" customHeight="1">
       <c r="A5" s="7" t="s">
         <v>3</v>
       </c>
@@ -3910,10 +3913,10 @@
       <c r="D5" s="10">
         <v>-3.5600812999999998</v>
       </c>
-      <c r="E5" s="26"/>
-      <c r="F5" s="65"/>
-    </row>
-    <row r="6" spans="1:12" s="32" customFormat="1" ht="20" customHeight="1">
+      <c r="E5" s="24"/>
+      <c r="F5" s="54"/>
+    </row>
+    <row r="6" spans="1:12" s="30" customFormat="1" ht="20" customHeight="1">
       <c r="A6" s="7" t="s">
         <v>4</v>
       </c>
@@ -3926,10 +3929,10 @@
       <c r="D6" s="10">
         <v>-4.5210676999999997</v>
       </c>
-      <c r="E6" s="26"/>
-      <c r="F6" s="65"/>
-    </row>
-    <row r="7" spans="1:12" s="32" customFormat="1" ht="20" customHeight="1">
+      <c r="E6" s="24"/>
+      <c r="F6" s="54"/>
+    </row>
+    <row r="7" spans="1:12" s="30" customFormat="1" ht="20" customHeight="1">
       <c r="A7" s="7" t="s">
         <v>5</v>
       </c>
@@ -3942,10 +3945,10 @@
       <c r="D7" s="10">
         <v>-8.3079698000000004</v>
       </c>
-      <c r="E7" s="26"/>
-      <c r="F7" s="65"/>
-    </row>
-    <row r="8" spans="1:12" s="32" customFormat="1" ht="20" customHeight="1">
+      <c r="E7" s="24"/>
+      <c r="F7" s="54"/>
+    </row>
+    <row r="8" spans="1:12" s="30" customFormat="1" ht="20" customHeight="1">
       <c r="A8" s="7" t="s">
         <v>6</v>
       </c>
@@ -3958,10 +3961,10 @@
       <c r="D8" s="10">
         <v>-11.3453512</v>
       </c>
-      <c r="E8" s="26"/>
-      <c r="F8" s="65"/>
-    </row>
-    <row r="9" spans="1:12" s="32" customFormat="1" ht="20" customHeight="1">
+      <c r="E8" s="24"/>
+      <c r="F8" s="54"/>
+    </row>
+    <row r="9" spans="1:12" s="30" customFormat="1" ht="20" customHeight="1">
       <c r="A9" s="7" t="s">
         <v>7</v>
       </c>
@@ -3974,57 +3977,57 @@
       <c r="D9" s="10">
         <v>-14.2877314</v>
       </c>
-      <c r="E9" s="26"/>
-      <c r="F9" s="65"/>
-    </row>
-    <row r="10" spans="1:12" s="32" customFormat="1" ht="20" customHeight="1">
+      <c r="E9" s="24"/>
+      <c r="F9" s="54"/>
+    </row>
+    <row r="10" spans="1:12" s="30" customFormat="1" ht="20" customHeight="1">
       <c r="A10" s="7"/>
       <c r="B10" s="11"/>
       <c r="C10" s="12"/>
       <c r="D10" s="12"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="65"/>
-    </row>
-    <row r="11" spans="1:12" s="32" customFormat="1" ht="20" customHeight="1">
+      <c r="E10" s="25"/>
+      <c r="F10" s="54"/>
+    </row>
+    <row r="11" spans="1:12" s="30" customFormat="1" ht="20" customHeight="1">
       <c r="A11" s="14"/>
-      <c r="B11" s="77" t="s">
+      <c r="B11" s="78" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="69"/>
-      <c r="D11" s="70"/>
-      <c r="E11" s="71"/>
-      <c r="F11" s="65"/>
-    </row>
-    <row r="12" spans="1:12" s="32" customFormat="1" ht="104" customHeight="1">
-      <c r="A12" s="76" t="s">
+      <c r="C11" s="79"/>
+      <c r="D11" s="80"/>
+      <c r="E11" s="55"/>
+      <c r="F11" s="54"/>
+    </row>
+    <row r="12" spans="1:12" s="30" customFormat="1" ht="104" customHeight="1">
+      <c r="A12" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="79" t="s">
+      <c r="B12" s="88" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="80"/>
-      <c r="D12" s="74"/>
-      <c r="E12" s="75"/>
-    </row>
-    <row r="13" spans="1:12" s="32" customFormat="1" ht="20" customHeight="1">
+      <c r="C12" s="89"/>
+      <c r="D12" s="86"/>
+      <c r="E12" s="87"/>
+    </row>
+    <row r="13" spans="1:12" s="30" customFormat="1" ht="20" customHeight="1">
       <c r="A13" s="13"/>
-      <c r="B13" s="78"/>
-      <c r="C13" s="72"/>
-      <c r="D13" s="72"/>
-      <c r="E13" s="73"/>
-      <c r="F13" s="65"/>
-    </row>
-    <row r="14" spans="1:12" s="32" customFormat="1" ht="20" customHeight="1">
+      <c r="B13" s="59"/>
+      <c r="C13" s="56"/>
+      <c r="D13" s="56"/>
+      <c r="E13" s="57"/>
+      <c r="F13" s="54"/>
+    </row>
+    <row r="14" spans="1:12" s="30" customFormat="1" ht="20" customHeight="1">
       <c r="A14" s="14"/>
-      <c r="B14" s="66" t="s">
+      <c r="B14" s="83" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="67"/>
-      <c r="D14" s="68"/>
+      <c r="C14" s="84"/>
+      <c r="D14" s="85"/>
       <c r="E14" s="14"/>
-      <c r="F14" s="65"/>
-    </row>
-    <row r="15" spans="1:12" s="32" customFormat="1" ht="20" customHeight="1">
+      <c r="F14" s="54"/>
+    </row>
+    <row r="15" spans="1:12" s="30" customFormat="1" ht="20" customHeight="1">
       <c r="A15" s="13"/>
       <c r="B15" s="19" t="s">
         <v>12</v>
@@ -4035,12 +4038,12 @@
       <c r="D15" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="28" t="s">
+      <c r="E15" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="F15" s="65"/>
-    </row>
-    <row r="16" spans="1:12" s="32" customFormat="1" ht="20" customHeight="1">
+      <c r="F15" s="54"/>
+    </row>
+    <row r="16" spans="1:12" s="30" customFormat="1" ht="20" customHeight="1">
       <c r="A16" s="7" t="s">
         <v>16</v>
       </c>
@@ -4053,12 +4056,12 @@
       <c r="D16" s="10">
         <v>75.026480000000006</v>
       </c>
-      <c r="E16" s="29">
+      <c r="E16" s="27">
         <v>28211</v>
       </c>
-      <c r="F16" s="65"/>
-    </row>
-    <row r="17" spans="1:6" s="32" customFormat="1" ht="20" customHeight="1">
+      <c r="F16" s="54"/>
+    </row>
+    <row r="17" spans="1:6" s="30" customFormat="1" ht="20" customHeight="1">
       <c r="A17" s="7" t="s">
         <v>2</v>
       </c>
@@ -4071,12 +4074,12 @@
       <c r="D17" s="10">
         <v>66.83511</v>
       </c>
-      <c r="E17" s="29">
+      <c r="E17" s="27">
         <v>59351</v>
       </c>
-      <c r="F17" s="65"/>
-    </row>
-    <row r="18" spans="1:6" s="32" customFormat="1" ht="20" customHeight="1">
+      <c r="F17" s="54"/>
+    </row>
+    <row r="18" spans="1:6" s="30" customFormat="1" ht="20" customHeight="1">
       <c r="A18" s="7" t="s">
         <v>3</v>
       </c>
@@ -4089,12 +4092,12 @@
       <c r="D18" s="10">
         <v>63.716839999999998</v>
       </c>
-      <c r="E18" s="29">
+      <c r="E18" s="27">
         <v>90094</v>
       </c>
-      <c r="F18" s="65"/>
-    </row>
-    <row r="19" spans="1:6" s="32" customFormat="1" ht="20" customHeight="1">
+      <c r="F18" s="54"/>
+    </row>
+    <row r="19" spans="1:6" s="30" customFormat="1" ht="20" customHeight="1">
       <c r="A19" s="7" t="s">
         <v>4</v>
       </c>
@@ -4107,12 +4110,12 @@
       <c r="D19" s="10">
         <v>83.606279999999998</v>
       </c>
-      <c r="E19" s="29">
+      <c r="E19" s="27">
         <v>132316</v>
       </c>
-      <c r="F19" s="65"/>
-    </row>
-    <row r="20" spans="1:6" s="32" customFormat="1" ht="20" customHeight="1">
+      <c r="F19" s="54"/>
+    </row>
+    <row r="20" spans="1:6" s="30" customFormat="1" ht="20" customHeight="1">
       <c r="A20" s="7" t="s">
         <v>5</v>
       </c>
@@ -4125,12 +4128,12 @@
       <c r="D20" s="10">
         <v>51.091650000000001</v>
       </c>
-      <c r="E20" s="29">
+      <c r="E20" s="27">
         <v>125630</v>
       </c>
-      <c r="F20" s="65"/>
-    </row>
-    <row r="21" spans="1:6" s="32" customFormat="1" ht="20" customHeight="1">
+      <c r="F20" s="54"/>
+    </row>
+    <row r="21" spans="1:6" s="30" customFormat="1" ht="20" customHeight="1">
       <c r="A21" s="7" t="s">
         <v>6</v>
       </c>
@@ -4143,41 +4146,41 @@
       <c r="D21" s="10">
         <v>43.939109999999999</v>
       </c>
-      <c r="E21" s="29">
+      <c r="E21" s="27">
         <v>96367</v>
       </c>
-      <c r="F21" s="65"/>
-    </row>
-    <row r="22" spans="1:6" s="32" customFormat="1" ht="20" customHeight="1">
-      <c r="A22" s="60" t="s">
+      <c r="F21" s="54"/>
+    </row>
+    <row r="22" spans="1:6" s="30" customFormat="1" ht="20" customHeight="1">
+      <c r="A22" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="B22" s="61">
+      <c r="B22" s="50">
         <v>48.961689999999997</v>
       </c>
-      <c r="C22" s="62">
+      <c r="C22" s="51">
         <v>36</v>
       </c>
-      <c r="D22" s="62">
+      <c r="D22" s="51">
         <v>36.958350000000003</v>
       </c>
-      <c r="E22" s="63">
+      <c r="E22" s="52">
         <v>5873</v>
       </c>
-      <c r="F22" s="65"/>
-    </row>
-    <row r="23" spans="1:6" s="32" customFormat="1" ht="20" customHeight="1">
-      <c r="A23" s="56"/>
-      <c r="B23" s="57"/>
-      <c r="C23" s="57"/>
-      <c r="D23" s="57"/>
-      <c r="E23" s="57"/>
-    </row>
-    <row r="24" spans="1:6" s="32" customFormat="1" ht="20" customHeight="1">
-      <c r="A24" s="31"/>
-    </row>
-    <row r="25" spans="1:6" s="32" customFormat="1" ht="20" customHeight="1">
-      <c r="A25" s="31"/>
+      <c r="F22" s="54"/>
+    </row>
+    <row r="23" spans="1:6" s="30" customFormat="1" ht="20" customHeight="1">
+      <c r="A23" s="47"/>
+      <c r="B23" s="48"/>
+      <c r="C23" s="48"/>
+      <c r="D23" s="48"/>
+      <c r="E23" s="48"/>
+    </row>
+    <row r="24" spans="1:6" s="30" customFormat="1" ht="20" customHeight="1">
+      <c r="A24" s="29"/>
+    </row>
+    <row r="25" spans="1:6" s="30" customFormat="1" ht="20" customHeight="1">
+      <c r="A25" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -4212,555 +4215,555 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="20.46484375" style="50" customWidth="1"/>
-    <col min="2" max="13" width="16.33203125" style="50" customWidth="1"/>
-    <col min="14" max="256" width="16.33203125" style="32" customWidth="1"/>
-    <col min="257" max="16384" width="16.33203125" style="32"/>
+    <col min="1" max="1" width="20.46484375" style="44" customWidth="1"/>
+    <col min="2" max="13" width="16.33203125" style="44" customWidth="1"/>
+    <col min="14" max="256" width="16.33203125" style="30" customWidth="1"/>
+    <col min="257" max="16384" width="16.33203125" style="30"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" customFormat="1" ht="27.75" customHeight="1">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="95" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="23"/>
+      <c r="B1" s="95"/>
+      <c r="C1" s="95"/>
+      <c r="D1" s="95"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
     </row>
     <row r="2" spans="1:13" customFormat="1" ht="32.25" customHeight="1">
-      <c r="A2" s="34"/>
-      <c r="B2" s="35" t="s">
+      <c r="A2" s="32"/>
+      <c r="B2" s="93" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
+      <c r="C2" s="94"/>
+      <c r="D2" s="94"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
     </row>
     <row r="3" spans="1:13" customFormat="1" ht="20.25" customHeight="1" thickBot="1">
-      <c r="A3" s="37"/>
-      <c r="B3" s="46">
+      <c r="A3" s="33"/>
+      <c r="B3" s="42">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="C3" s="47" t="s">
+      <c r="C3" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="46">
+      <c r="D3" s="42">
         <v>0.97499999999999998</v>
       </c>
-      <c r="E3" s="38"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="32"/>
-      <c r="L3" s="32"/>
-      <c r="M3" s="32"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="30"/>
+      <c r="L3" s="30"/>
+      <c r="M3" s="30"/>
     </row>
     <row r="4" spans="1:13" customFormat="1" ht="20" customHeight="1">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="44">
+      <c r="B4" s="40">
         <v>369.18365</v>
       </c>
-      <c r="C4" s="45">
+      <c r="C4" s="41">
         <v>380.95</v>
       </c>
-      <c r="D4" s="44">
+      <c r="D4" s="40">
         <v>392.70686000000001</v>
       </c>
-      <c r="E4" s="38"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="32"/>
-      <c r="H4" s="32"/>
-      <c r="I4" s="32"/>
-      <c r="J4" s="32"/>
-      <c r="K4" s="32"/>
-      <c r="L4" s="32"/>
-      <c r="M4" s="32"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="30"/>
+      <c r="K4" s="30"/>
+      <c r="L4" s="30"/>
+      <c r="M4" s="30"/>
     </row>
     <row r="5" spans="1:13" customFormat="1" ht="20" customHeight="1">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="40">
+      <c r="B5" s="36">
         <v>-54.24277</v>
       </c>
-      <c r="C5" s="41">
+      <c r="C5" s="37">
         <v>-39.97</v>
       </c>
-      <c r="D5" s="40">
+      <c r="D5" s="36">
         <v>-25.695879999999999</v>
       </c>
-      <c r="E5" s="38"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="32"/>
-      <c r="I5" s="32"/>
-      <c r="J5" s="32"/>
-      <c r="K5" s="32"/>
-      <c r="L5" s="32"/>
-      <c r="M5" s="32"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="30"/>
+      <c r="I5" s="30"/>
+      <c r="J5" s="30"/>
+      <c r="K5" s="30"/>
+      <c r="L5" s="30"/>
+      <c r="M5" s="30"/>
     </row>
     <row r="6" spans="1:13" customFormat="1" ht="20" customHeight="1">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="40">
+      <c r="B6" s="36">
         <v>-92.580560000000006</v>
       </c>
-      <c r="C6" s="41">
+      <c r="C6" s="37">
         <v>-79.2</v>
       </c>
-      <c r="D6" s="40">
+      <c r="D6" s="36">
         <v>-65.813990000000004</v>
       </c>
-      <c r="E6" s="38"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="32"/>
-      <c r="I6" s="32"/>
-      <c r="J6" s="32"/>
-      <c r="K6" s="32"/>
-      <c r="L6" s="32"/>
-      <c r="M6" s="32"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="30"/>
+      <c r="K6" s="30"/>
+      <c r="L6" s="30"/>
+      <c r="M6" s="30"/>
     </row>
     <row r="7" spans="1:13" customFormat="1" ht="20" customHeight="1">
-      <c r="A7" s="39" t="s">
+      <c r="A7" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="40">
+      <c r="B7" s="36">
         <v>-124.25714000000001</v>
       </c>
-      <c r="C7" s="41">
+      <c r="C7" s="37">
         <v>-111.38</v>
       </c>
-      <c r="D7" s="40">
+      <c r="D7" s="36">
         <v>-98.494699999999995</v>
       </c>
-      <c r="E7" s="38"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="32"/>
-      <c r="I7" s="32"/>
-      <c r="J7" s="32"/>
-      <c r="K7" s="32"/>
-      <c r="L7" s="32"/>
-      <c r="M7" s="32"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="30"/>
+      <c r="I7" s="30"/>
+      <c r="J7" s="30"/>
+      <c r="K7" s="30"/>
+      <c r="L7" s="30"/>
+      <c r="M7" s="30"/>
     </row>
     <row r="8" spans="1:13" customFormat="1" ht="20" customHeight="1">
-      <c r="A8" s="39" t="s">
+      <c r="A8" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="40">
+      <c r="B8" s="36">
         <v>-153.93755999999999</v>
       </c>
-      <c r="C8" s="41">
+      <c r="C8" s="37">
         <v>-141.07</v>
       </c>
-      <c r="D8" s="40">
+      <c r="D8" s="36">
         <v>-128.18268</v>
       </c>
-      <c r="E8" s="38"/>
-      <c r="F8" s="32"/>
-      <c r="G8" s="32"/>
-      <c r="H8" s="32"/>
-      <c r="I8" s="32"/>
-      <c r="J8" s="32"/>
-      <c r="K8" s="32"/>
-      <c r="L8" s="32"/>
-      <c r="M8" s="32"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="30"/>
+      <c r="I8" s="30"/>
+      <c r="J8" s="30"/>
+      <c r="K8" s="30"/>
+      <c r="L8" s="30"/>
+      <c r="M8" s="30"/>
     </row>
     <row r="9" spans="1:13" customFormat="1" ht="20" customHeight="1">
-      <c r="A9" s="39" t="s">
+      <c r="A9" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="40">
+      <c r="B9" s="36">
         <v>-179.71325999999999</v>
       </c>
-      <c r="C9" s="41">
+      <c r="C9" s="37">
         <v>-166.52</v>
       </c>
-      <c r="D9" s="40">
+      <c r="D9" s="36">
         <v>-153.32028</v>
       </c>
-      <c r="E9" s="38"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="32"/>
-      <c r="H9" s="32"/>
-      <c r="I9" s="32"/>
-      <c r="J9" s="32"/>
-      <c r="K9" s="32"/>
-      <c r="L9" s="32"/>
-      <c r="M9" s="32"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="30"/>
+      <c r="H9" s="30"/>
+      <c r="I9" s="30"/>
+      <c r="J9" s="30"/>
+      <c r="K9" s="30"/>
+      <c r="L9" s="30"/>
+      <c r="M9" s="30"/>
     </row>
     <row r="10" spans="1:13" customFormat="1" ht="20" customHeight="1">
-      <c r="A10" s="39" t="s">
+      <c r="A10" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="40">
+      <c r="B10" s="36">
         <v>-234.95685</v>
       </c>
-      <c r="C10" s="41">
+      <c r="C10" s="37">
         <v>-206.54</v>
       </c>
-      <c r="D10" s="40">
+      <c r="D10" s="36">
         <v>-178.10865999999999</v>
       </c>
-      <c r="E10" s="38"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32"/>
-      <c r="H10" s="32"/>
-      <c r="I10" s="32"/>
-      <c r="J10" s="32"/>
-      <c r="K10" s="32"/>
-      <c r="L10" s="32"/>
-      <c r="M10" s="32"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="30"/>
+      <c r="J10" s="30"/>
+      <c r="K10" s="30"/>
+      <c r="L10" s="30"/>
+      <c r="M10" s="30"/>
     </row>
     <row r="11" spans="1:13" customFormat="1" ht="20" customHeight="1">
-      <c r="A11" s="39"/>
-      <c r="B11" s="42"/>
-      <c r="C11" s="42"/>
-      <c r="D11" s="42"/>
-      <c r="E11" s="42"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="32"/>
-      <c r="H11" s="32"/>
-      <c r="I11" s="32"/>
-      <c r="J11" s="32"/>
-      <c r="K11" s="32"/>
-      <c r="L11" s="32"/>
-      <c r="M11" s="32"/>
+      <c r="A11" s="35"/>
+      <c r="B11" s="38"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="30"/>
+      <c r="H11" s="30"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="30"/>
+      <c r="K11" s="30"/>
+      <c r="L11" s="30"/>
+      <c r="M11" s="30"/>
     </row>
     <row r="12" spans="1:13" customFormat="1" ht="20" customHeight="1">
-      <c r="A12" s="34"/>
-      <c r="B12" s="51" t="s">
+      <c r="A12" s="32"/>
+      <c r="B12" s="90" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="52"/>
-      <c r="D12" s="53"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="32"/>
-      <c r="H12" s="32"/>
-      <c r="I12" s="32"/>
-      <c r="J12" s="32"/>
-      <c r="K12" s="32"/>
-      <c r="L12" s="32"/>
-      <c r="M12" s="32"/>
+      <c r="C12" s="91"/>
+      <c r="D12" s="92"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="30"/>
+      <c r="H12" s="30"/>
+      <c r="I12" s="30"/>
+      <c r="J12" s="30"/>
+      <c r="K12" s="30"/>
+      <c r="L12" s="30"/>
+      <c r="M12" s="30"/>
     </row>
     <row r="13" spans="1:13" customFormat="1" ht="104" customHeight="1">
-      <c r="A13" s="89" t="s">
+      <c r="A13" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="48" t="s">
+      <c r="B13" s="97" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="49"/>
-      <c r="D13" s="48"/>
-      <c r="E13" s="49"/>
-      <c r="F13" s="32"/>
-      <c r="G13" s="32"/>
-      <c r="H13" s="32"/>
-      <c r="I13" s="32"/>
-      <c r="J13" s="32"/>
-      <c r="K13" s="32"/>
-      <c r="L13" s="32"/>
-      <c r="M13" s="32"/>
+      <c r="C13" s="98"/>
+      <c r="D13" s="97"/>
+      <c r="E13" s="98"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="30"/>
+      <c r="I13" s="30"/>
+      <c r="J13" s="30"/>
+      <c r="K13" s="30"/>
+      <c r="L13" s="30"/>
+      <c r="M13" s="30"/>
     </row>
     <row r="14" spans="1:13" customFormat="1" ht="20" customHeight="1">
-      <c r="A14" s="37"/>
-      <c r="B14" s="38"/>
-      <c r="C14" s="38"/>
-      <c r="D14" s="38"/>
-      <c r="E14" s="38"/>
-      <c r="F14" s="32"/>
-      <c r="G14" s="32"/>
-      <c r="H14" s="32"/>
-      <c r="I14" s="32"/>
-      <c r="J14" s="32"/>
-      <c r="K14" s="32"/>
-      <c r="L14" s="32"/>
-      <c r="M14" s="32"/>
+      <c r="A14" s="33"/>
+      <c r="B14" s="34"/>
+      <c r="C14" s="34"/>
+      <c r="D14" s="34"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="30"/>
+      <c r="J14" s="30"/>
+      <c r="K14" s="30"/>
+      <c r="L14" s="30"/>
+      <c r="M14" s="30"/>
     </row>
     <row r="15" spans="1:13" customFormat="1" ht="20" customHeight="1">
-      <c r="A15" s="34"/>
-      <c r="B15" s="51" t="s">
+      <c r="A15" s="32"/>
+      <c r="B15" s="90" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="52"/>
-      <c r="D15" s="53"/>
-      <c r="E15" s="34"/>
-      <c r="F15" s="32"/>
-      <c r="G15" s="32"/>
-      <c r="H15" s="32"/>
-      <c r="I15" s="32"/>
-      <c r="J15" s="32"/>
-      <c r="K15" s="32"/>
-      <c r="L15" s="32"/>
-      <c r="M15" s="32"/>
+      <c r="C15" s="91"/>
+      <c r="D15" s="92"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="30"/>
+      <c r="J15" s="30"/>
+      <c r="K15" s="30"/>
+      <c r="L15" s="30"/>
+      <c r="M15" s="30"/>
     </row>
     <row r="16" spans="1:13" customFormat="1" ht="32" customHeight="1">
-      <c r="A16" s="37"/>
-      <c r="B16" s="43" t="s">
+      <c r="A16" s="33"/>
+      <c r="B16" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="43" t="s">
+      <c r="C16" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="D16" s="43" t="s">
+      <c r="D16" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="E16" s="43" t="s">
+      <c r="E16" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="F16" s="32"/>
-      <c r="G16" s="33" t="s">
+      <c r="F16" s="30"/>
+      <c r="G16" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="H16" s="32"/>
-      <c r="I16" s="32"/>
-      <c r="J16" s="32"/>
-      <c r="K16" s="32"/>
-      <c r="L16" s="32"/>
-      <c r="M16" s="32"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="30"/>
+      <c r="J16" s="30"/>
+      <c r="K16" s="30"/>
+      <c r="L16" s="30"/>
+      <c r="M16" s="30"/>
     </row>
     <row r="17" spans="1:13" customFormat="1" ht="20" customHeight="1">
-      <c r="A17" s="39" t="s">
+      <c r="A17" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="40">
+      <c r="B17" s="36">
         <v>346.06</v>
       </c>
-      <c r="C17" s="40">
+      <c r="C17" s="36">
         <v>216</v>
       </c>
-      <c r="D17" s="40">
+      <c r="D17" s="36">
         <v>431.49</v>
       </c>
-      <c r="E17" s="40">
+      <c r="E17" s="36">
         <v>32842</v>
       </c>
-      <c r="F17" s="32"/>
-      <c r="G17" s="32"/>
-      <c r="H17" s="32"/>
-      <c r="I17" s="32"/>
-      <c r="J17" s="32"/>
-      <c r="K17" s="32"/>
-      <c r="L17" s="32"/>
-      <c r="M17" s="32"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="30"/>
+      <c r="J17" s="30"/>
+      <c r="K17" s="30"/>
+      <c r="L17" s="30"/>
+      <c r="M17" s="30"/>
     </row>
     <row r="18" spans="1:13" customFormat="1" ht="20" customHeight="1">
-      <c r="A18" s="39" t="s">
+      <c r="A18" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="40">
+      <c r="B18" s="36">
         <v>309.51</v>
       </c>
-      <c r="C18" s="40">
+      <c r="C18" s="36">
         <v>192</v>
       </c>
-      <c r="D18" s="40">
+      <c r="D18" s="36">
         <v>400.68</v>
       </c>
-      <c r="E18" s="40">
+      <c r="E18" s="36">
         <v>80805</v>
       </c>
-      <c r="F18" s="32"/>
-      <c r="G18" s="32"/>
-      <c r="H18" s="32"/>
-      <c r="I18" s="32"/>
-      <c r="J18" s="32"/>
-      <c r="K18" s="32"/>
-      <c r="L18" s="32"/>
-      <c r="M18" s="32"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="30"/>
+      <c r="H18" s="30"/>
+      <c r="I18" s="30"/>
+      <c r="J18" s="30"/>
+      <c r="K18" s="30"/>
+      <c r="L18" s="30"/>
+      <c r="M18" s="30"/>
     </row>
     <row r="19" spans="1:13" customFormat="1" ht="20" customHeight="1">
-      <c r="A19" s="39" t="s">
+      <c r="A19" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="B19" s="40">
+      <c r="B19" s="36">
         <v>279.33</v>
       </c>
-      <c r="C19" s="40">
+      <c r="C19" s="36">
         <v>180</v>
       </c>
-      <c r="D19" s="40">
+      <c r="D19" s="36">
         <v>354.61</v>
       </c>
-      <c r="E19" s="40">
+      <c r="E19" s="36">
         <v>142523</v>
       </c>
-      <c r="F19" s="32"/>
-      <c r="G19" s="32"/>
-      <c r="H19" s="32"/>
-      <c r="I19" s="32"/>
-      <c r="J19" s="32"/>
-      <c r="K19" s="32"/>
-      <c r="L19" s="32"/>
-      <c r="M19" s="32"/>
+      <c r="F19" s="30"/>
+      <c r="G19" s="30"/>
+      <c r="H19" s="30"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
+      <c r="K19" s="30"/>
+      <c r="L19" s="30"/>
+      <c r="M19" s="30"/>
     </row>
     <row r="20" spans="1:13" customFormat="1" ht="20" customHeight="1">
-      <c r="A20" s="39" t="s">
+      <c r="A20" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="B20" s="40">
+      <c r="B20" s="36">
         <v>250.5</v>
       </c>
-      <c r="C20" s="40">
+      <c r="C20" s="36">
         <v>160</v>
       </c>
-      <c r="D20" s="40">
+      <c r="D20" s="36">
         <v>319.37</v>
       </c>
-      <c r="E20" s="40">
+      <c r="E20" s="36">
         <v>234291</v>
       </c>
-      <c r="F20" s="32"/>
-      <c r="G20" s="32"/>
-      <c r="H20" s="32"/>
-      <c r="I20" s="32"/>
-      <c r="J20" s="32"/>
-      <c r="K20" s="32"/>
-      <c r="L20" s="32"/>
-      <c r="M20" s="32"/>
+      <c r="F20" s="30"/>
+      <c r="G20" s="30"/>
+      <c r="H20" s="30"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="30"/>
+      <c r="K20" s="30"/>
+      <c r="L20" s="30"/>
+      <c r="M20" s="30"/>
     </row>
     <row r="21" spans="1:13" customFormat="1" ht="20" customHeight="1">
-      <c r="A21" s="39" t="s">
+      <c r="A21" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="B21" s="40">
+      <c r="B21" s="36">
         <v>221.24</v>
       </c>
-      <c r="C21" s="40">
+      <c r="C21" s="36">
         <v>144</v>
       </c>
-      <c r="D21" s="40">
+      <c r="D21" s="36">
         <v>294.27</v>
       </c>
-      <c r="E21" s="40">
+      <c r="E21" s="36">
         <v>258781</v>
       </c>
-      <c r="F21" s="32"/>
-      <c r="G21" s="32"/>
-      <c r="H21" s="32"/>
-      <c r="I21" s="32"/>
-      <c r="J21" s="32"/>
-      <c r="K21" s="32"/>
-      <c r="L21" s="32"/>
-      <c r="M21" s="32"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="30"/>
+      <c r="H21" s="30"/>
+      <c r="I21" s="30"/>
+      <c r="J21" s="30"/>
+      <c r="K21" s="30"/>
+      <c r="L21" s="30"/>
+      <c r="M21" s="30"/>
     </row>
     <row r="22" spans="1:13" customFormat="1" ht="20" customHeight="1">
-      <c r="A22" s="39" t="s">
+      <c r="A22" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="B22" s="40">
+      <c r="B22" s="36">
         <v>196.83</v>
       </c>
-      <c r="C22" s="40">
+      <c r="C22" s="36">
         <v>124</v>
       </c>
-      <c r="D22" s="40">
+      <c r="D22" s="36">
         <v>262.52999999999997</v>
       </c>
-      <c r="E22" s="40">
+      <c r="E22" s="36">
         <v>226407</v>
       </c>
-      <c r="F22" s="32"/>
-      <c r="G22" s="32"/>
-      <c r="H22" s="32"/>
-      <c r="I22" s="32"/>
-      <c r="J22" s="32"/>
-      <c r="K22" s="32"/>
-      <c r="L22" s="32"/>
-      <c r="M22" s="32"/>
+      <c r="F22" s="30"/>
+      <c r="G22" s="30"/>
+      <c r="H22" s="30"/>
+      <c r="I22" s="30"/>
+      <c r="J22" s="30"/>
+      <c r="K22" s="30"/>
+      <c r="L22" s="30"/>
+      <c r="M22" s="30"/>
     </row>
     <row r="23" spans="1:13" customFormat="1" ht="20" customHeight="1">
-      <c r="A23" s="54" t="s">
+      <c r="A23" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="B23" s="55">
+      <c r="B23" s="46">
         <v>165.06</v>
       </c>
-      <c r="C23" s="55">
+      <c r="C23" s="46">
         <v>112</v>
       </c>
-      <c r="D23" s="55">
+      <c r="D23" s="46">
         <v>224.43</v>
       </c>
-      <c r="E23" s="55">
+      <c r="E23" s="46">
         <v>16500</v>
       </c>
-      <c r="F23" s="32"/>
-      <c r="G23" s="32"/>
-      <c r="H23" s="32"/>
-      <c r="I23" s="32"/>
-      <c r="J23" s="32"/>
-      <c r="K23" s="32"/>
-      <c r="L23" s="32"/>
-      <c r="M23" s="32"/>
+      <c r="F23" s="30"/>
+      <c r="G23" s="30"/>
+      <c r="H23" s="30"/>
+      <c r="I23" s="30"/>
+      <c r="J23" s="30"/>
+      <c r="K23" s="30"/>
+      <c r="L23" s="30"/>
+      <c r="M23" s="30"/>
     </row>
     <row r="24" spans="1:13" customFormat="1" ht="20" customHeight="1">
-      <c r="A24" s="56"/>
-      <c r="B24" s="57"/>
-      <c r="C24" s="57"/>
-      <c r="D24" s="57"/>
-      <c r="E24" s="57"/>
-      <c r="F24" s="32"/>
-      <c r="G24" s="32"/>
-      <c r="H24" s="32"/>
-      <c r="I24" s="32"/>
-      <c r="J24" s="32"/>
-      <c r="K24" s="32"/>
-      <c r="L24" s="32"/>
-      <c r="M24" s="32"/>
+      <c r="A24" s="47"/>
+      <c r="B24" s="48"/>
+      <c r="C24" s="48"/>
+      <c r="D24" s="48"/>
+      <c r="E24" s="48"/>
+      <c r="F24" s="30"/>
+      <c r="G24" s="30"/>
+      <c r="H24" s="30"/>
+      <c r="I24" s="30"/>
+      <c r="J24" s="30"/>
+      <c r="K24" s="30"/>
+      <c r="L24" s="30"/>
+      <c r="M24" s="30"/>
     </row>
     <row r="25" spans="1:13" customFormat="1" ht="20" customHeight="1">
-      <c r="A25" s="31"/>
-      <c r="B25" s="32"/>
-      <c r="C25" s="32"/>
-      <c r="D25" s="32"/>
-      <c r="E25" s="32"/>
-      <c r="F25" s="32"/>
-      <c r="G25" s="32"/>
-      <c r="H25" s="32"/>
-      <c r="I25" s="32"/>
-      <c r="J25" s="32"/>
-      <c r="K25" s="32"/>
-      <c r="L25" s="32"/>
-      <c r="M25" s="32"/>
+      <c r="A25" s="29"/>
+      <c r="B25" s="30"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="30"/>
+      <c r="F25" s="30"/>
+      <c r="G25" s="30"/>
+      <c r="H25" s="30"/>
+      <c r="I25" s="30"/>
+      <c r="J25" s="30"/>
+      <c r="K25" s="30"/>
+      <c r="L25" s="30"/>
+      <c r="M25" s="30"/>
     </row>
     <row r="26" spans="1:13" customFormat="1" ht="20" customHeight="1">
-      <c r="A26" s="31"/>
-      <c r="B26" s="32"/>
-      <c r="C26" s="32"/>
-      <c r="D26" s="32"/>
-      <c r="E26" s="32"/>
-      <c r="F26" s="32"/>
-      <c r="G26" s="32"/>
-      <c r="H26" s="32"/>
-      <c r="I26" s="32"/>
-      <c r="J26" s="32"/>
-      <c r="K26" s="32"/>
-      <c r="L26" s="32"/>
-      <c r="M26" s="32"/>
+      <c r="A26" s="29"/>
+      <c r="B26" s="30"/>
+      <c r="C26" s="30"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="30"/>
+      <c r="F26" s="30"/>
+      <c r="G26" s="30"/>
+      <c r="H26" s="30"/>
+      <c r="I26" s="30"/>
+      <c r="J26" s="30"/>
+      <c r="K26" s="30"/>
+      <c r="L26" s="30"/>
+      <c r="M26" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -4803,168 +4806,168 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="27.75" customHeight="1">
-      <c r="A1" s="81" t="s">
+      <c r="A1" s="99" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="81"/>
-      <c r="C1" s="81"/>
-      <c r="D1" s="81"/>
-      <c r="E1" s="81"/>
+      <c r="B1" s="99"/>
+      <c r="C1" s="99"/>
+      <c r="D1" s="99"/>
+      <c r="E1" s="99"/>
     </row>
     <row r="2" spans="1:5" ht="27.75" customHeight="1">
-      <c r="A2" s="34"/>
-      <c r="B2" s="51" t="s">
+      <c r="A2" s="32"/>
+      <c r="B2" s="90" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="52"/>
-      <c r="D2" s="53"/>
+      <c r="C2" s="91"/>
+      <c r="D2" s="92"/>
       <c r="E2" s="16"/>
     </row>
     <row r="3" spans="1:5" ht="20.25" customHeight="1">
-      <c r="A3" s="87" t="s">
+      <c r="A3" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="88" t="s">
+      <c r="B3" s="66" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="88" t="s">
+      <c r="C3" s="66" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="88" t="s">
+      <c r="D3" s="66" t="s">
         <v>24</v>
       </c>
       <c r="E3" s="17"/>
     </row>
     <row r="4" spans="1:5" ht="20.25" customHeight="1">
-      <c r="A4" s="82" t="s">
+      <c r="A4" s="60" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="83">
+      <c r="B4" s="61">
         <v>24.487819999999999</v>
       </c>
-      <c r="C4" s="83">
+      <c r="C4" s="61">
         <v>0.77493999999999996</v>
       </c>
-      <c r="D4" s="83">
+      <c r="D4" s="61">
         <v>31.599699999999999</v>
       </c>
       <c r="E4" s="15"/>
     </row>
     <row r="5" spans="1:5" ht="20" customHeight="1">
-      <c r="A5" s="82" t="s">
+      <c r="A5" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="83">
+      <c r="B5" s="61">
         <v>0.65622999999999998</v>
       </c>
-      <c r="C5" s="83">
+      <c r="C5" s="61">
         <v>0.93413000000000002</v>
       </c>
-      <c r="D5" s="83">
+      <c r="D5" s="61">
         <v>0.70250000000000001</v>
       </c>
       <c r="E5" s="15"/>
     </row>
     <row r="6" spans="1:5" ht="20" customHeight="1">
-      <c r="A6" s="82" t="s">
+      <c r="A6" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="83">
+      <c r="B6" s="61">
         <v>-0.47986000000000001</v>
       </c>
-      <c r="C6" s="83">
+      <c r="C6" s="61">
         <v>0.87431999999999999</v>
       </c>
-      <c r="D6" s="83">
+      <c r="D6" s="61">
         <v>-0.54879999999999995</v>
       </c>
       <c r="E6" s="15"/>
     </row>
     <row r="7" spans="1:5" ht="20" customHeight="1">
-      <c r="A7" s="82" t="s">
+      <c r="A7" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="83">
+      <c r="B7" s="61">
         <v>-2.8964400000000001</v>
       </c>
-      <c r="C7" s="83">
+      <c r="C7" s="61">
         <v>0.84187999999999996</v>
       </c>
-      <c r="D7" s="83">
+      <c r="D7" s="61">
         <v>-3.4403999999999999</v>
       </c>
       <c r="E7" s="15"/>
     </row>
     <row r="8" spans="1:5" ht="20" customHeight="1">
-      <c r="A8" s="82" t="s">
+      <c r="A8" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="83">
+      <c r="B8" s="61">
         <v>-5.8544299999999998</v>
       </c>
-      <c r="C8" s="83">
+      <c r="C8" s="61">
         <v>0.84016999999999997</v>
       </c>
-      <c r="D8" s="83">
+      <c r="D8" s="61">
         <v>-6.9682000000000004</v>
       </c>
       <c r="E8" s="15"/>
     </row>
     <row r="9" spans="1:5" ht="20" customHeight="1">
-      <c r="A9" s="82" t="s">
+      <c r="A9" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="83">
+      <c r="B9" s="61">
         <v>-9.0466499999999996</v>
       </c>
-      <c r="C9" s="83">
+      <c r="C9" s="61">
         <v>0.85706000000000004</v>
       </c>
-      <c r="D9" s="83">
+      <c r="D9" s="61">
         <v>-10.555400000000001</v>
       </c>
       <c r="E9" s="15"/>
     </row>
     <row r="10" spans="1:5" ht="20" customHeight="1">
-      <c r="A10" s="82" t="s">
+      <c r="A10" s="60" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="83">
+      <c r="B10" s="61">
         <v>-13.81015</v>
       </c>
-      <c r="C10" s="83">
+      <c r="C10" s="61">
         <v>1.7251700000000001</v>
       </c>
-      <c r="D10" s="83">
+      <c r="D10" s="61">
         <v>-8.0051000000000005</v>
       </c>
       <c r="E10" s="15"/>
     </row>
     <row r="11" spans="1:5" ht="20" customHeight="1">
-      <c r="A11" s="39"/>
-      <c r="B11" s="84"/>
-      <c r="C11" s="84"/>
-      <c r="D11" s="84"/>
+      <c r="A11" s="35"/>
+      <c r="B11" s="62"/>
+      <c r="C11" s="62"/>
+      <c r="D11" s="62"/>
       <c r="E11" s="15"/>
     </row>
     <row r="12" spans="1:5" ht="13.15">
-      <c r="A12" s="34"/>
-      <c r="B12" s="51" t="s">
+      <c r="A12" s="32"/>
+      <c r="B12" s="90" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="52"/>
-      <c r="D12" s="52"/>
-      <c r="E12" s="64"/>
+      <c r="C12" s="91"/>
+      <c r="D12" s="91"/>
+      <c r="E12" s="53"/>
     </row>
     <row r="13" spans="1:5" ht="127.15" customHeight="1">
-      <c r="A13" s="89" t="s">
+      <c r="A13" s="67" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="83" t="s">
+      <c r="B13" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="85"/>
-      <c r="D13" s="86"/>
+      <c r="C13" s="63"/>
+      <c r="D13" s="64"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4991,174 +4994,174 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="16.265625" style="32" customWidth="1"/>
-    <col min="2" max="2" width="24" style="32" customWidth="1"/>
-    <col min="3" max="3" width="21.19921875" style="32" customWidth="1"/>
-    <col min="4" max="4" width="23.46484375" style="32" customWidth="1"/>
-    <col min="5" max="16384" width="10.6640625" style="32"/>
+    <col min="1" max="1" width="16.265625" style="30" customWidth="1"/>
+    <col min="2" max="2" width="24" style="30" customWidth="1"/>
+    <col min="3" max="3" width="21.19921875" style="30" customWidth="1"/>
+    <col min="4" max="4" width="23.46484375" style="30" customWidth="1"/>
+    <col min="5" max="16384" width="10.6640625" style="30"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" customHeight="1">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="100" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="92"/>
-      <c r="C1" s="92"/>
-      <c r="D1" s="93"/>
-      <c r="E1" s="103"/>
+      <c r="B1" s="101"/>
+      <c r="C1" s="101"/>
+      <c r="D1" s="102"/>
+      <c r="E1" s="75"/>
     </row>
     <row r="2" spans="1:5" ht="12.75" customHeight="1">
-      <c r="A2" s="94"/>
-      <c r="B2" s="90"/>
-      <c r="C2" s="90"/>
-      <c r="D2" s="95"/>
-      <c r="E2" s="103"/>
+      <c r="A2" s="103"/>
+      <c r="B2" s="104"/>
+      <c r="C2" s="104"/>
+      <c r="D2" s="105"/>
+      <c r="E2" s="75"/>
     </row>
     <row r="3" spans="1:5" ht="13.15">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="51" t="s">
+      <c r="B3" s="90" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="52"/>
-      <c r="D3" s="53"/>
+      <c r="C3" s="91"/>
+      <c r="D3" s="92"/>
     </row>
     <row r="4" spans="1:5" ht="20" customHeight="1">
-      <c r="A4" s="82" t="s">
+      <c r="A4" s="60" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="96" t="s">
+      <c r="B4" s="68" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="96" t="s">
+      <c r="C4" s="68" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="97" t="s">
+      <c r="D4" s="69" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="20" customHeight="1">
-      <c r="A5" s="82" t="s">
+      <c r="A5" s="60" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="98" t="s">
+      <c r="B5" s="70" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="99">
+      <c r="C5" s="71">
         <v>1.1032999999999999</v>
       </c>
-      <c r="D5" s="100">
+      <c r="D5" s="72">
         <v>84.433000000000007</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="20" customHeight="1">
-      <c r="A6" s="82">
+      <c r="A6" s="60">
         <v>2</v>
       </c>
-      <c r="B6" s="99">
+      <c r="B6" s="71">
         <v>-13.899800000000001</v>
       </c>
-      <c r="C6" s="99">
+      <c r="C6" s="71">
         <v>1.3395999999999999</v>
       </c>
-      <c r="D6" s="100">
+      <c r="D6" s="72">
         <v>-10.375999999999999</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="20" customHeight="1">
-      <c r="A7" s="82">
+      <c r="A7" s="60">
         <v>3</v>
       </c>
-      <c r="B7" s="99">
+      <c r="B7" s="71">
         <v>-21.3611</v>
       </c>
-      <c r="C7" s="99">
+      <c r="C7" s="71">
         <v>1.256</v>
       </c>
-      <c r="D7" s="100">
+      <c r="D7" s="72">
         <v>-17.007000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="20" customHeight="1">
-      <c r="A8" s="82">
+      <c r="A8" s="60">
         <v>4</v>
       </c>
-      <c r="B8" s="99">
+      <c r="B8" s="71">
         <v>-30.212399999999999</v>
       </c>
-      <c r="C8" s="99">
+      <c r="C8" s="71">
         <v>1.2088000000000001</v>
       </c>
-      <c r="D8" s="100">
+      <c r="D8" s="72">
         <v>-24.994</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="20" customHeight="1">
-      <c r="A9" s="82">
+      <c r="A9" s="60">
         <v>5</v>
       </c>
-      <c r="B9" s="99">
+      <c r="B9" s="71">
         <v>-38.918700000000001</v>
       </c>
-      <c r="C9" s="99">
+      <c r="C9" s="71">
         <v>1.2084999999999999</v>
       </c>
-      <c r="D9" s="100">
+      <c r="D9" s="72">
         <v>-32.206000000000003</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="20" customHeight="1">
-      <c r="A10" s="82">
+      <c r="A10" s="60">
         <v>6</v>
       </c>
-      <c r="B10" s="98" t="s">
+      <c r="B10" s="70" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="99">
+      <c r="C10" s="71">
         <v>1.2384999999999999</v>
       </c>
-      <c r="D10" s="100">
+      <c r="D10" s="72">
         <v>-37.256999999999998</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="20" customHeight="1">
-      <c r="A11" s="82">
+      <c r="A11" s="60">
         <v>7</v>
       </c>
-      <c r="B11" s="99">
+      <c r="B11" s="71">
         <v>-55.047400000000003</v>
       </c>
-      <c r="C11" s="99">
+      <c r="C11" s="71">
         <v>2.6709000000000001</v>
       </c>
-      <c r="D11" s="100">
+      <c r="D11" s="72">
         <v>-20.61</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="20" customHeight="1">
-      <c r="A12" s="82"/>
-      <c r="B12" s="30"/>
-      <c r="C12" s="30"/>
-      <c r="D12" s="101"/>
+      <c r="A12" s="60"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="73"/>
     </row>
     <row r="13" spans="1:5" ht="31.9" customHeight="1">
-      <c r="A13" s="34"/>
-      <c r="B13" s="51" t="s">
+      <c r="A13" s="32"/>
+      <c r="B13" s="90" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="52"/>
-      <c r="D13" s="53"/>
+      <c r="C13" s="91"/>
+      <c r="D13" s="92"/>
     </row>
     <row r="14" spans="1:5" ht="127.15" customHeight="1">
-      <c r="A14" s="89" t="s">
+      <c r="A14" s="67" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="104" t="s">
+      <c r="B14" s="76" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="74"/>
-      <c r="D14" s="75"/>
+      <c r="C14" s="86"/>
+      <c r="D14" s="87"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -5177,167 +5180,167 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:D12"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="17.73046875" customWidth="1"/>
-    <col min="2" max="3" width="20.6640625" style="32" customWidth="1"/>
-    <col min="4" max="4" width="20.19921875" style="32" customWidth="1"/>
-    <col min="5" max="16384" width="10.6640625" style="32"/>
+    <col min="1" max="1" width="17.73046875" style="28" customWidth="1"/>
+    <col min="2" max="3" width="20.6640625" style="30" customWidth="1"/>
+    <col min="4" max="4" width="20.19921875" style="30" customWidth="1"/>
+    <col min="5" max="16384" width="10.6640625" style="30"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="100" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="92"/>
-      <c r="C1" s="92"/>
-      <c r="D1" s="93"/>
+      <c r="B1" s="101"/>
+      <c r="C1" s="101"/>
+      <c r="D1" s="102"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="94"/>
-      <c r="B2" s="90"/>
-      <c r="C2" s="90"/>
-      <c r="D2" s="95"/>
+      <c r="A2" s="103"/>
+      <c r="B2" s="104"/>
+      <c r="C2" s="104"/>
+      <c r="D2" s="105"/>
     </row>
     <row r="3" spans="1:5" ht="20" customHeight="1">
-      <c r="A3" s="87" t="s">
+      <c r="A3" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="96" t="s">
+      <c r="B3" s="68" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="96" t="s">
+      <c r="C3" s="68" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="97" t="s">
+      <c r="D3" s="69" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="20" customHeight="1">
-      <c r="A4" s="82" t="s">
+      <c r="A4" s="60" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="99">
+      <c r="B4" s="71">
         <v>782.16</v>
       </c>
-      <c r="C4" s="99">
+      <c r="C4" s="71">
         <v>11.234999999999999</v>
       </c>
-      <c r="D4" s="100">
+      <c r="D4" s="72">
         <v>69.617000000000004</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="20" customHeight="1">
-      <c r="A5" s="82">
+      <c r="A5" s="60">
         <v>2</v>
       </c>
-      <c r="B5" s="99">
+      <c r="B5" s="71">
         <v>-164.53899999999999</v>
       </c>
-      <c r="C5" s="99">
+      <c r="C5" s="71">
         <v>13.646000000000001</v>
       </c>
-      <c r="D5" s="100">
+      <c r="D5" s="72">
         <v>-12.058</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="20" customHeight="1">
-      <c r="A6" s="82">
+      <c r="A6" s="60">
         <v>3</v>
       </c>
-      <c r="B6" s="99">
+      <c r="B6" s="71">
         <v>-243.572</v>
       </c>
-      <c r="C6" s="99">
+      <c r="C6" s="71">
         <v>12.798</v>
       </c>
-      <c r="D6" s="100">
+      <c r="D6" s="72">
         <v>-19.033000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="20" customHeight="1">
-      <c r="A7" s="82">
+      <c r="A7" s="60">
         <v>4</v>
       </c>
-      <c r="B7" s="99">
+      <c r="B7" s="71">
         <v>-318.78699999999998</v>
       </c>
-      <c r="C7" s="99">
+      <c r="C7" s="71">
         <v>12.316000000000001</v>
       </c>
-      <c r="D7" s="100">
+      <c r="D7" s="72">
         <v>-25.882999999999999</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="20" customHeight="1">
-      <c r="A8" s="82">
+      <c r="A8" s="60">
         <v>5</v>
       </c>
-      <c r="B8" s="99">
+      <c r="B8" s="71">
         <v>-388.96100000000001</v>
       </c>
-      <c r="C8" s="99">
+      <c r="C8" s="71">
         <v>12.314</v>
       </c>
-      <c r="D8" s="100">
+      <c r="D8" s="72">
         <v>-31.587</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="20" customHeight="1">
-      <c r="A9" s="82">
+      <c r="A9" s="60">
         <v>6</v>
       </c>
-      <c r="B9" s="99">
+      <c r="B9" s="71">
         <v>-437.19299999999998</v>
       </c>
-      <c r="C9" s="99">
+      <c r="C9" s="71">
         <v>12.624000000000001</v>
       </c>
-      <c r="D9" s="100">
+      <c r="D9" s="72">
         <v>-34.631999999999998</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="20" customHeight="1">
-      <c r="A10" s="82">
+      <c r="A10" s="60">
         <v>7</v>
       </c>
-      <c r="B10" s="99">
+      <c r="B10" s="71">
         <v>-487.77499999999998</v>
       </c>
-      <c r="C10" s="99">
+      <c r="C10" s="71">
         <v>27.38</v>
       </c>
-      <c r="D10" s="100">
+      <c r="D10" s="72">
         <v>-17.815000000000001</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="20" customHeight="1">
-      <c r="A11" s="82"/>
-      <c r="B11" s="30"/>
-      <c r="C11" s="30"/>
-      <c r="D11" s="101"/>
+      <c r="A11" s="60"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="73"/>
     </row>
     <row r="12" spans="1:5" ht="78.75" customHeight="1">
-      <c r="A12" s="34"/>
-      <c r="B12" s="105" t="s">
+      <c r="A12" s="32"/>
+      <c r="B12" s="106" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="106"/>
+      <c r="C12" s="107"/>
       <c r="D12" s="108"/>
-      <c r="E12" s="107"/>
+      <c r="E12" s="77"/>
     </row>
     <row r="13" spans="1:5" ht="122.25" customHeight="1">
-      <c r="A13" s="87" t="s">
+      <c r="A13" s="110" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="102" t="s">
+      <c r="B13" s="74" t="s">
         <v>10</v>
       </c>
       <c r="C13" s="109"/>
-      <c r="D13" s="75"/>
+      <c r="D13" s="87"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>